<commit_message>
actualizar seminarios e hitos
</commit_message>
<xml_diff>
--- a/input_hitos.xlsx
+++ b/input_hitos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elenaqb/Documents/PROJECTS/new_website/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elenaqb/Documents/Cursos/EcoInformatica/new_website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFCB1EB5-CBB4-9A48-9055-110E8FF54E0F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{449998E1-2CFE-1C44-9B41-50D9BBD5D891}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36640" yWindow="-4780" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="36620" yWindow="-4780" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="83">
   <si>
     <t>month</t>
   </si>
@@ -288,6 +288,18 @@
   </si>
   <si>
     <t>https://doi.org/10.7818/ECOS.2016.25-1.17</t>
+  </si>
+  <si>
+    <t>https://youtu.be/ck6rzzSy4kE</t>
+  </si>
+  <si>
+    <t>https://youtu.be/K94y_zAGLmc?si=CWGMofxry_pUcRt6</t>
+  </si>
+  <si>
+    <t>Análisis de textos con R: ejemplos útiles para la ecología</t>
+  </si>
+  <si>
+    <t>OCCUR Shiny app: flujo de trabajo para validar registros de especies</t>
   </si>
 </sst>
 </file>
@@ -332,11 +344,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -623,10 +638,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -634,6 +649,7 @@
     <col min="2" max="2" width="19.6640625" customWidth="1"/>
     <col min="3" max="3" width="38.5" customWidth="1"/>
     <col min="4" max="4" width="45.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="43" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -1255,8 +1271,42 @@
       <c r="D37" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="E37" s="2" t="s">
+      <c r="E37" s="3" t="s">
         <v>77</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="112" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>2</v>
+      </c>
+      <c r="B38">
+        <v>2025</v>
+      </c>
+      <c r="C38" t="s">
+        <v>5</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="160" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>4</v>
+      </c>
+      <c r="B39">
+        <v>2025</v>
+      </c>
+      <c r="C39" t="s">
+        <v>5</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1286,6 +1336,8 @@
     <hyperlink ref="D17" r:id="rId20" xr:uid="{FD95CFC5-9A2D-4FBE-87B2-2338AE65BEFB}"/>
     <hyperlink ref="D23" r:id="rId21" xr:uid="{60288E13-EF5B-4C40-8C1D-869D1FCD4AF3}"/>
     <hyperlink ref="D37" r:id="rId22" xr:uid="{EC2B4E9A-8AEC-4854-A5D0-63A4DFFFF640}"/>
+    <hyperlink ref="D39" r:id="rId23" xr:uid="{810D07BB-5DAD-7048-94C6-F22CA9C69D1C}"/>
+    <hyperlink ref="D38" r:id="rId24" xr:uid="{96BD9742-6D56-D648-BA34-D75C77BB1CF9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
nav bar colours, ecoinformatics notes as menu and hitos meetings #8
</commit_message>
<xml_diff>
--- a/input_hitos.xlsx
+++ b/input_hitos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elenaqb/Documents/Cursos/EcoInformatica/new_website/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UNI\6. SEVILLA\99. OTROS\9999. TERMINADOS\2024_11_19 WEB Ecoinformatica\new_website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{449998E1-2CFE-1C44-9B41-50D9BBD5D891}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62164A17-CD36-41D9-96A3-7DF58C80CDC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36620" yWindow="-4780" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="85">
   <si>
     <t>month</t>
   </si>
@@ -300,6 +300,12 @@
   </si>
   <si>
     <t>OCCUR Shiny app: flujo de trabajo para validar registros de especies</t>
+  </si>
+  <si>
+    <t>Reunión del grupo Almería</t>
+  </si>
+  <si>
+    <t>Reunión del grupo Pontevedra</t>
   </si>
 </sst>
 </file>
@@ -369,10 +375,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -638,21 +640,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E39"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="H39" sqref="H39"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.6640625" customWidth="1"/>
-    <col min="3" max="3" width="38.5" customWidth="1"/>
-    <col min="4" max="4" width="45.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" customWidth="1"/>
+    <col min="3" max="3" width="38.42578125" customWidth="1"/>
+    <col min="4" max="4" width="45.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="43" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -669,7 +671,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -683,7 +685,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="160" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
@@ -700,7 +702,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="160" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>6</v>
       </c>
@@ -717,7 +719,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="112" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>11</v>
       </c>
@@ -734,7 +736,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="208" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
@@ -751,7 +753,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="192" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>7</v>
       </c>
@@ -768,7 +770,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="192" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -785,7 +787,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="144" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>3</v>
       </c>
@@ -802,7 +804,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>11</v>
       </c>
@@ -819,7 +821,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2</v>
       </c>
@@ -836,7 +838,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="144" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -853,7 +855,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>5</v>
       </c>
@@ -870,7 +872,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="144" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -887,7 +889,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="128" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>6</v>
       </c>
@@ -904,7 +906,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="96" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>12</v>
       </c>
@@ -921,7 +923,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="208" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2</v>
       </c>
@@ -938,26 +940,22 @@
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="288" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
+        <v>10</v>
+      </c>
+      <c r="B18">
+        <v>2023</v>
+      </c>
+      <c r="C18" t="s">
+        <v>83</v>
+      </c>
+      <c r="D18" s="1"/>
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A19">
         <v>6</v>
-      </c>
-      <c r="B18">
-        <v>2024</v>
-      </c>
-      <c r="C18" t="s">
-        <v>25</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="112" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>8</v>
       </c>
       <c r="B19">
         <v>2024</v>
@@ -965,47 +963,47 @@
       <c r="C19" t="s">
         <v>25</v>
       </c>
-      <c r="D19" t="s">
-        <v>19</v>
+      <c r="D19" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B20">
         <v>2024</v>
       </c>
       <c r="C20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" t="s">
+        <v>19</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>10</v>
+      </c>
+      <c r="B21">
+        <v>2024</v>
+      </c>
+      <c r="C21" t="s">
         <v>4</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D21" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="96" x14ac:dyDescent="0.2">
-      <c r="A21">
+    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22">
         <v>1</v>
-      </c>
-      <c r="B21">
-        <v>2022</v>
-      </c>
-      <c r="C21" t="s">
-        <v>5</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>2</v>
       </c>
       <c r="B22">
         <v>2022</v>
@@ -1014,15 +1012,15 @@
         <v>5</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="160" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B23">
         <v>2022</v>
@@ -1031,15 +1029,15 @@
         <v>5</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="96" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B24">
         <v>2022</v>
@@ -1047,16 +1045,16 @@
       <c r="C24" t="s">
         <v>5</v>
       </c>
-      <c r="D24" t="s">
-        <v>28</v>
+      <c r="D24" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="96" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B25">
         <v>2022</v>
@@ -1065,15 +1063,15 @@
         <v>5</v>
       </c>
       <c r="D25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B26">
         <v>2022</v>
@@ -1082,15 +1080,15 @@
         <v>5</v>
       </c>
       <c r="D26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="144" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B27">
         <v>2022</v>
@@ -1099,15 +1097,15 @@
         <v>5</v>
       </c>
       <c r="D27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="112" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B28">
         <v>2022</v>
@@ -1116,15 +1114,15 @@
         <v>5</v>
       </c>
       <c r="D28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="96" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B29">
         <v>2022</v>
@@ -1133,32 +1131,32 @@
         <v>5</v>
       </c>
       <c r="D29" t="s">
+        <v>32</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>11</v>
+      </c>
+      <c r="B30">
+        <v>2022</v>
+      </c>
+      <c r="C30" t="s">
+        <v>5</v>
+      </c>
+      <c r="D30" t="s">
         <v>33</v>
       </c>
-      <c r="E29" s="2" t="s">
+      <c r="E30" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A30">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31">
         <v>3</v>
-      </c>
-      <c r="B30">
-        <v>2023</v>
-      </c>
-      <c r="C30" t="s">
-        <v>5</v>
-      </c>
-      <c r="D30" t="s">
-        <v>34</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="64" x14ac:dyDescent="0.2">
-      <c r="A31">
-        <v>5</v>
       </c>
       <c r="B31">
         <v>2023</v>
@@ -1167,15 +1165,15 @@
         <v>5</v>
       </c>
       <c r="D31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="96" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B32">
         <v>2023</v>
@@ -1184,32 +1182,32 @@
         <v>5</v>
       </c>
       <c r="D32" t="s">
+        <v>35</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>9</v>
+      </c>
+      <c r="B33">
+        <v>2023</v>
+      </c>
+      <c r="C33" t="s">
+        <v>5</v>
+      </c>
+      <c r="D33" t="s">
         <v>36</v>
       </c>
-      <c r="E32" s="2" t="s">
+      <c r="E33" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="96" x14ac:dyDescent="0.2">
-      <c r="A33">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34">
         <v>1</v>
-      </c>
-      <c r="B33">
-        <v>2024</v>
-      </c>
-      <c r="C33" t="s">
-        <v>5</v>
-      </c>
-      <c r="D33" t="s">
-        <v>37</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="128" x14ac:dyDescent="0.2">
-      <c r="A34">
-        <v>3</v>
       </c>
       <c r="B34">
         <v>2024</v>
@@ -1218,15 +1216,15 @@
         <v>5</v>
       </c>
       <c r="D34" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="128" x14ac:dyDescent="0.2">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B35">
         <v>2024</v>
@@ -1235,15 +1233,15 @@
         <v>5</v>
       </c>
       <c r="D35" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="144" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B36">
         <v>2024</v>
@@ -1252,32 +1250,32 @@
         <v>5</v>
       </c>
       <c r="D36" t="s">
+        <v>39</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>5</v>
+      </c>
+      <c r="B37">
+        <v>2024</v>
+      </c>
+      <c r="C37" t="s">
+        <v>5</v>
+      </c>
+      <c r="D37" t="s">
         <v>40</v>
       </c>
-      <c r="E36" s="2" t="s">
+      <c r="E37" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="224" x14ac:dyDescent="0.2">
-      <c r="A37">
+    <row r="38" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A38">
         <v>1</v>
-      </c>
-      <c r="B37">
-        <v>2025</v>
-      </c>
-      <c r="C37" t="s">
-        <v>5</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="112" x14ac:dyDescent="0.2">
-      <c r="A38">
-        <v>2</v>
       </c>
       <c r="B38">
         <v>2025</v>
@@ -1286,15 +1284,15 @@
         <v>5</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="160" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B39">
         <v>2025</v>
@@ -1303,20 +1301,48 @@
         <v>5</v>
       </c>
       <c r="D39" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>4</v>
+      </c>
+      <c r="B40">
+        <v>2025</v>
+      </c>
+      <c r="C40" t="s">
+        <v>5</v>
+      </c>
+      <c r="D40" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E39" s="2" t="s">
+      <c r="E40" s="2" t="s">
         <v>82</v>
       </c>
     </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>6</v>
+      </c>
+      <c r="B41">
+        <v>2025</v>
+      </c>
+      <c r="C41" t="s">
+        <v>84</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="A2:E36">
-    <sortCondition ref="C1:C36"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E37">
+    <sortCondition ref="C1:C37"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="D3" r:id="rId1" xr:uid="{B5274820-F334-49F2-9C65-BC403D5350B7}"/>
     <hyperlink ref="D2" r:id="rId2" xr:uid="{6EBAFA3B-B2F0-45F6-951F-4D8B1064B063}"/>
-    <hyperlink ref="D20" r:id="rId3" xr:uid="{CF71B0EE-DA39-43CB-83C1-1A7ACCD20076}"/>
+    <hyperlink ref="D21" r:id="rId3" xr:uid="{CF71B0EE-DA39-43CB-83C1-1A7ACCD20076}"/>
     <hyperlink ref="D4" r:id="rId4" xr:uid="{C2C6E6B2-539C-400F-A20B-9060CA9373B6}"/>
     <hyperlink ref="D6" r:id="rId5" xr:uid="{E1B381D2-8052-4C8B-97B3-311E59DE5F30}"/>
     <hyperlink ref="D5" r:id="rId6" xr:uid="{78437E75-9C9E-48F9-A0D3-8ACA414C68AB}"/>
@@ -1327,17 +1353,17 @@
     <hyperlink ref="D13" r:id="rId11" xr:uid="{8577162C-E63C-4ACC-9C95-C5B28E37C309}"/>
     <hyperlink ref="D14" r:id="rId12" xr:uid="{398E5209-9D76-492C-BFCE-B4626DE88147}"/>
     <hyperlink ref="D16" r:id="rId13" xr:uid="{45E7E255-BDE5-4896-A1CA-B06330880EA8}"/>
-    <hyperlink ref="D18" r:id="rId14" xr:uid="{8BE493EC-DD6E-42D1-9EF8-C3DA113C4CF7}"/>
-    <hyperlink ref="D21" r:id="rId15" xr:uid="{8DCACB60-4B90-4A39-B11A-2A2A474761F8}"/>
-    <hyperlink ref="D22" r:id="rId16" xr:uid="{E8E2B09A-039D-4925-8081-7F92AC13837B}"/>
+    <hyperlink ref="D19" r:id="rId14" xr:uid="{8BE493EC-DD6E-42D1-9EF8-C3DA113C4CF7}"/>
+    <hyperlink ref="D22" r:id="rId15" xr:uid="{8DCACB60-4B90-4A39-B11A-2A2A474761F8}"/>
+    <hyperlink ref="D23" r:id="rId16" xr:uid="{E8E2B09A-039D-4925-8081-7F92AC13837B}"/>
     <hyperlink ref="D10" r:id="rId17" xr:uid="{35204F6C-7389-41C7-8CF4-B711F7A915A7}"/>
     <hyperlink ref="D12" r:id="rId18" xr:uid="{A930F9F4-CD0D-4330-BDFE-F6F1753610CC}"/>
     <hyperlink ref="D15" r:id="rId19" xr:uid="{A85240B0-C8E7-45A1-A9AB-B8E15A972011}"/>
     <hyperlink ref="D17" r:id="rId20" xr:uid="{FD95CFC5-9A2D-4FBE-87B2-2338AE65BEFB}"/>
-    <hyperlink ref="D23" r:id="rId21" xr:uid="{60288E13-EF5B-4C40-8C1D-869D1FCD4AF3}"/>
-    <hyperlink ref="D37" r:id="rId22" xr:uid="{EC2B4E9A-8AEC-4854-A5D0-63A4DFFFF640}"/>
-    <hyperlink ref="D39" r:id="rId23" xr:uid="{810D07BB-5DAD-7048-94C6-F22CA9C69D1C}"/>
-    <hyperlink ref="D38" r:id="rId24" xr:uid="{96BD9742-6D56-D648-BA34-D75C77BB1CF9}"/>
+    <hyperlink ref="D24" r:id="rId21" xr:uid="{60288E13-EF5B-4C40-8C1D-869D1FCD4AF3}"/>
+    <hyperlink ref="D38" r:id="rId22" xr:uid="{EC2B4E9A-8AEC-4854-A5D0-63A4DFFFF640}"/>
+    <hyperlink ref="D40" r:id="rId23" xr:uid="{810D07BB-5DAD-7048-94C6-F22CA9C69D1C}"/>
+    <hyperlink ref="D39" r:id="rId24" xr:uid="{96BD9742-6D56-D648-BA34-D75C77BB1CF9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>